<commit_message>
Updated progress for 1.18
</commit_message>
<xml_diff>
--- a/kubernetes/Progress.xlsx
+++ b/kubernetes/Progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiming/work/SchemaStore/kubernetes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF452DB6-5776-1542-9C20-732EDCA3B857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C86BE70-53EA-ED48-8F08-1B77F63B2D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="6" xr2:uid="{2CA22A3D-9E43-5D48-92D2-AD75BE8904C6}"/>
   </bookViews>
@@ -19,7 +19,8 @@
     <sheet name="res-1.15" sheetId="5" r:id="rId4"/>
     <sheet name="res-1.16" sheetId="6" r:id="rId5"/>
     <sheet name="res-1.17" sheetId="7" r:id="rId6"/>
-    <sheet name="NameRules" sheetId="8" r:id="rId7"/>
+    <sheet name="res-1.18" sheetId="9" r:id="rId7"/>
+    <sheet name="NameRules" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2843" uniqueCount="754">
   <si>
     <t>name</t>
   </si>
@@ -2492,6 +2493,12 @@
   </si>
   <si>
     <t>a DNS-1123 subdomain must consist of lower case alphanumeric characters, '-' or '.', and must start and end with an alphanumeric character</t>
+  </si>
+  <si>
+    <t>StorageClass, VolumeAttachment, CSIDriver</t>
+  </si>
+  <si>
+    <t>Ingress, IngressClass</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2647,247 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="152">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9011,80 +9258,80 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="127" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="1" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="16" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="150" priority="16" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C93">
-    <cfRule type="containsText" dxfId="125" priority="15" operator="containsText" text="Deprecate">
+    <cfRule type="containsText" dxfId="149" priority="15" operator="containsText" text="Deprecate">
       <formula>NOT(ISERROR(SEARCH("Deprecate",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C383">
-    <cfRule type="containsText" dxfId="124" priority="14" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="148" priority="14" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C383)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C385:C397">
-    <cfRule type="containsText" dxfId="123" priority="13" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="147" priority="13" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C385)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C418:C420">
-    <cfRule type="containsText" dxfId="122" priority="12" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="146" priority="12" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C418)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C411:C417">
-    <cfRule type="containsText" dxfId="121" priority="11" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="145" priority="11" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C411)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C421:C425">
-    <cfRule type="containsText" dxfId="120" priority="10" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="144" priority="10" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C421)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C398">
-    <cfRule type="containsText" dxfId="119" priority="9" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="143" priority="9" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C398)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C429">
-    <cfRule type="containsText" dxfId="118" priority="8" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="142" priority="8" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C429)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C430">
-    <cfRule type="containsText" dxfId="117" priority="7" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="141" priority="7" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C430)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C431">
-    <cfRule type="containsText" dxfId="116" priority="6" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="140" priority="6" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C431)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C435">
-    <cfRule type="containsText" dxfId="115" priority="5" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="139" priority="5" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C435)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C401">
-    <cfRule type="containsText" dxfId="114" priority="4" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="138" priority="4" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C401)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C402:C403">
-    <cfRule type="containsText" dxfId="113" priority="3" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="137" priority="3" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C402)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C384">
-    <cfRule type="containsText" dxfId="112" priority="2" operator="containsText" text="Deprecated">
+    <cfRule type="containsText" dxfId="136" priority="2" operator="containsText" text="Deprecated">
       <formula>NOT(ISERROR(SEARCH("Deprecated",C384)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9916,18 +10163,18 @@
     <sortCondition ref="A2:A36"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576 F23">
-    <cfRule type="cellIs" dxfId="111" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F36">
-    <cfRule type="cellIs" dxfId="109" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10871,66 +11118,66 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F24 E1:E27 E31:E34 E36:E1048576">
-    <cfRule type="cellIs" dxfId="107" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="16" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F27 F31:F34 F36:F41">
-    <cfRule type="cellIs" dxfId="105" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="14" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28 E30">
-    <cfRule type="cellIs" dxfId="103" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="12" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28 F30:G30">
-    <cfRule type="cellIs" dxfId="101" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="99" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="93" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11873,66 +12120,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F24 E1:E27 E31:E34 E36:E1048576">
-    <cfRule type="cellIs" dxfId="91" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="16" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F27 F31:F34 F36:F41">
-    <cfRule type="cellIs" dxfId="89" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="14" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28 E30">
-    <cfRule type="cellIs" dxfId="87" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="12" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28 F30:G30">
-    <cfRule type="cellIs" dxfId="85" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="83" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="8" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="81" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12557,6 +12804,1109 @@
         <v>624</v>
       </c>
       <c r="G27" s="11" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>612</v>
+      </c>
+      <c r="B28" t="s">
+        <v>656</v>
+      </c>
+      <c r="C28" t="s">
+        <v>597</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>624</v>
+      </c>
+      <c r="F28" t="s">
+        <v>624</v>
+      </c>
+      <c r="G28" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>613</v>
+      </c>
+      <c r="B29" t="s">
+        <v>613</v>
+      </c>
+      <c r="C29" t="s">
+        <v>597</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>624</v>
+      </c>
+      <c r="F29" t="s">
+        <v>624</v>
+      </c>
+      <c r="G29" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>614</v>
+      </c>
+      <c r="B30" t="s">
+        <v>669</v>
+      </c>
+      <c r="C30" t="s">
+        <v>599</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>624</v>
+      </c>
+      <c r="F30" t="s">
+        <v>624</v>
+      </c>
+      <c r="G30" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>614</v>
+      </c>
+      <c r="B31" t="s">
+        <v>669</v>
+      </c>
+      <c r="C31" t="s">
+        <v>597</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>624</v>
+      </c>
+      <c r="F31" t="s">
+        <v>624</v>
+      </c>
+      <c r="G31" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>673</v>
+      </c>
+      <c r="B32" t="s">
+        <v>674</v>
+      </c>
+      <c r="C32" t="s">
+        <v>596</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>629</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>673</v>
+      </c>
+      <c r="B33" t="s">
+        <v>674</v>
+      </c>
+      <c r="C33" t="s">
+        <v>597</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>624</v>
+      </c>
+      <c r="F33" t="s">
+        <v>624</v>
+      </c>
+      <c r="G33" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>615</v>
+      </c>
+      <c r="B34" t="s">
+        <v>615</v>
+      </c>
+      <c r="C34" t="s">
+        <v>597</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>624</v>
+      </c>
+      <c r="F34" t="s">
+        <v>624</v>
+      </c>
+      <c r="G34" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>616</v>
+      </c>
+      <c r="B35" t="s">
+        <v>651</v>
+      </c>
+      <c r="C35" t="s">
+        <v>599</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>624</v>
+      </c>
+      <c r="F35" t="s">
+        <v>624</v>
+      </c>
+      <c r="G35" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>616</v>
+      </c>
+      <c r="B36" t="s">
+        <v>651</v>
+      </c>
+      <c r="C36" t="s">
+        <v>596</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>629</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>616</v>
+      </c>
+      <c r="B37" t="s">
+        <v>651</v>
+      </c>
+      <c r="C37" t="s">
+        <v>597</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>629</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>617</v>
+      </c>
+      <c r="B38" t="s">
+        <v>655</v>
+      </c>
+      <c r="C38" t="s">
+        <v>599</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>624</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="G38" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>617</v>
+      </c>
+      <c r="B39" t="s">
+        <v>655</v>
+      </c>
+      <c r="C39" t="s">
+        <v>596</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>629</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="10" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>617</v>
+      </c>
+      <c r="B40" t="s">
+        <v>655</v>
+      </c>
+      <c r="C40" t="s">
+        <v>597</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>624</v>
+      </c>
+      <c r="F40" t="s">
+        <v>624</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>618</v>
+      </c>
+      <c r="B41" t="s">
+        <v>657</v>
+      </c>
+      <c r="C41" t="s">
+        <v>596</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>624</v>
+      </c>
+      <c r="F41" t="s">
+        <v>624</v>
+      </c>
+      <c r="G41" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>619</v>
+      </c>
+      <c r="B42" t="s">
+        <v>670</v>
+      </c>
+      <c r="C42" t="s">
+        <v>599</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>624</v>
+      </c>
+      <c r="F42" t="s">
+        <v>624</v>
+      </c>
+      <c r="G42" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>619</v>
+      </c>
+      <c r="B43" t="s">
+        <v>670</v>
+      </c>
+      <c r="C43" t="s">
+        <v>596</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>629</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>619</v>
+      </c>
+      <c r="B44" t="s">
+        <v>670</v>
+      </c>
+      <c r="C44" t="s">
+        <v>597</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>629</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="F45" s="8"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F26:F27 E1:E2 E34:E37 E39:E1048576 E4 G27 E6:E30">
+    <cfRule type="cellIs" dxfId="99" priority="23" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="24" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2 F34:F37 F39:F44 F4 G27 F6:F30">
+    <cfRule type="cellIs" dxfId="97" priority="21" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="22" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31 E33">
+    <cfRule type="cellIs" dxfId="95" priority="19" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="20" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31 F33:G33">
+    <cfRule type="cellIs" dxfId="93" priority="17" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="18" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="91" priority="15" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="16" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" dxfId="89" priority="13" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="14" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="cellIs" dxfId="87" priority="11" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="12" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="cellIs" dxfId="85" priority="9" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="10" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="83" priority="7" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="8" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="81" priority="5" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="6" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06EC3E1A-DBD8-1D44-926E-239C341D46E6}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="186.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C3" t="s">
+        <v>599</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>624</v>
+      </c>
+      <c r="F3" t="s">
+        <v>624</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B4" t="s">
+        <v>652</v>
+      </c>
+      <c r="C4" t="s">
+        <v>597</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>624</v>
+      </c>
+      <c r="F4" t="s">
+        <v>624</v>
+      </c>
+      <c r="G4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>620</v>
+      </c>
+      <c r="B5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F5" t="s">
+        <v>624</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B6" t="s">
+        <v>664</v>
+      </c>
+      <c r="C6" t="s">
+        <v>597</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F6" t="s">
+        <v>624</v>
+      </c>
+      <c r="G6" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>621</v>
+      </c>
+      <c r="B7" t="s">
+        <v>665</v>
+      </c>
+      <c r="C7" t="s">
+        <v>599</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>624</v>
+      </c>
+      <c r="F7" t="s">
+        <v>624</v>
+      </c>
+      <c r="G7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>621</v>
+      </c>
+      <c r="B8" t="s">
+        <v>665</v>
+      </c>
+      <c r="C8" t="s">
+        <v>597</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>629</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>598</v>
+      </c>
+      <c r="B9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C9" t="s">
+        <v>599</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>624</v>
+      </c>
+      <c r="F9" t="s">
+        <v>624</v>
+      </c>
+      <c r="G9" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>598</v>
+      </c>
+      <c r="B10" t="s">
+        <v>598</v>
+      </c>
+      <c r="C10" t="s">
+        <v>597</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>629</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>598</v>
+      </c>
+      <c r="B11" t="s">
+        <v>598</v>
+      </c>
+      <c r="C11" t="s">
+        <v>600</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>629</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>601</v>
+      </c>
+      <c r="B12" t="s">
+        <v>653</v>
+      </c>
+      <c r="C12" t="s">
+        <v>596</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>624</v>
+      </c>
+      <c r="F12" t="s">
+        <v>624</v>
+      </c>
+      <c r="G12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>602</v>
+      </c>
+      <c r="B13" t="s">
+        <v>666</v>
+      </c>
+      <c r="C13" t="s">
+        <v>599</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>624</v>
+      </c>
+      <c r="F13" t="s">
+        <v>624</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>602</v>
+      </c>
+      <c r="B14" t="s">
+        <v>666</v>
+      </c>
+      <c r="C14" t="s">
+        <v>597</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>629</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>603</v>
+      </c>
+      <c r="B15" t="s">
+        <v>667</v>
+      </c>
+      <c r="C15" t="s">
+        <v>599</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>624</v>
+      </c>
+      <c r="F15" t="s">
+        <v>624</v>
+      </c>
+      <c r="G15" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>603</v>
+      </c>
+      <c r="B16" t="s">
+        <v>667</v>
+      </c>
+      <c r="C16" t="s">
+        <v>597</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>629</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>604</v>
+      </c>
+      <c r="B17" t="s">
+        <v>604</v>
+      </c>
+      <c r="C17" t="s">
+        <v>599</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>624</v>
+      </c>
+      <c r="F17" t="s">
+        <v>624</v>
+      </c>
+      <c r="G17" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>604</v>
+      </c>
+      <c r="B18" t="s">
+        <v>604</v>
+      </c>
+      <c r="C18" t="s">
+        <v>605</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>629</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>604</v>
+      </c>
+      <c r="B19" t="s">
+        <v>604</v>
+      </c>
+      <c r="C19" t="s">
+        <v>606</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>624</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="G19" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>607</v>
+      </c>
+      <c r="B20" t="s">
+        <v>607</v>
+      </c>
+      <c r="C20" t="s">
+        <v>599</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>624</v>
+      </c>
+      <c r="F20" t="s">
+        <v>624</v>
+      </c>
+      <c r="G20" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>607</v>
+      </c>
+      <c r="B21" t="s">
+        <v>607</v>
+      </c>
+      <c r="C21" t="s">
+        <v>597</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>624</v>
+      </c>
+      <c r="F21" t="s">
+        <v>624</v>
+      </c>
+      <c r="G21" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>607</v>
+      </c>
+      <c r="B22" t="s">
+        <v>607</v>
+      </c>
+      <c r="C22" t="s">
+        <v>608</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>629</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>609</v>
+      </c>
+      <c r="B23" t="s">
+        <v>654</v>
+      </c>
+      <c r="C23" t="s">
+        <v>597</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>624</v>
+      </c>
+      <c r="F23" t="s">
+        <v>624</v>
+      </c>
+      <c r="G23" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>610</v>
+      </c>
+      <c r="B24" t="s">
+        <v>668</v>
+      </c>
+      <c r="C24" t="s">
+        <v>599</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>624</v>
+      </c>
+      <c r="F24" t="s">
+        <v>624</v>
+      </c>
+      <c r="G24" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>610</v>
+      </c>
+      <c r="B25" t="s">
+        <v>668</v>
+      </c>
+      <c r="C25" t="s">
+        <v>597</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>624</v>
+      </c>
+      <c r="F25" t="s">
+        <v>624</v>
+      </c>
+      <c r="G25" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>611</v>
+      </c>
+      <c r="C26" t="s">
+        <v>599</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>624</v>
+      </c>
+      <c r="F26" t="s">
+        <v>624</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>681</v>
+      </c>
+      <c r="B27" t="s">
+        <v>682</v>
+      </c>
+      <c r="C27" t="s">
+        <v>596</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>624</v>
+      </c>
+      <c r="F27" t="s">
+        <v>624</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>683</v>
       </c>
     </row>
@@ -13043,12 +14393,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06EC3E1A-DBD8-1D44-926E-239C341D46E6}">
-  <dimension ref="A1:I45"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F7F6D4-3B59-1341-8861-F7C1EFC8DE2F}">
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="3" sqref="B1:B1048576 C1:C1048576 G1:G1048576 E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13085,24 +14435,26 @@
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="9" t="s">
+      <c r="A2" t="s">
         <v>592</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" t="s">
         <v>652</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>624</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>624</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>625</v>
+      <c r="C2" t="s">
+        <v>599</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>624</v>
+      </c>
+      <c r="F2" t="s">
+        <v>624</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -13113,7 +14465,7 @@
         <v>652</v>
       </c>
       <c r="C3" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -13124,22 +14476,22 @@
       <c r="F3" t="s">
         <v>624</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>686</v>
+      <c r="G3" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>592</v>
+        <v>620</v>
       </c>
       <c r="B4" t="s">
-        <v>652</v>
+        <v>664</v>
       </c>
       <c r="C4" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>624</v>
@@ -13147,8 +14499,8 @@
       <c r="F4" t="s">
         <v>624</v>
       </c>
-      <c r="G4" t="s">
-        <v>626</v>
+      <c r="G4" s="12" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -13159,7 +14511,7 @@
         <v>664</v>
       </c>
       <c r="C5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -13170,19 +14522,19 @@
       <c r="F5" t="s">
         <v>624</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B6" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C6" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -13194,7 +14546,7 @@
         <v>624</v>
       </c>
       <c r="G6" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -13205,54 +14557,54 @@
         <v>665</v>
       </c>
       <c r="C7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>624</v>
-      </c>
-      <c r="F7" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="G7" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
       <c r="B8" t="s">
-        <v>665</v>
+        <v>598</v>
       </c>
       <c r="C8" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>629</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F8" t="s">
+        <v>624</v>
+      </c>
       <c r="G8" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="B9" t="s">
-        <v>598</v>
+        <v>653</v>
       </c>
       <c r="C9" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>624</v>
@@ -13261,63 +14613,65 @@
         <v>624</v>
       </c>
       <c r="G9" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="B10" t="s">
-        <v>598</v>
+        <v>666</v>
       </c>
       <c r="C10" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>629</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" t="s">
-        <v>631</v>
+        <v>624</v>
+      </c>
+      <c r="F10" t="s">
+        <v>624</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="B11" t="s">
-        <v>598</v>
+        <v>666</v>
       </c>
       <c r="C11" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>629</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B12" t="s">
-        <v>653</v>
+        <v>667</v>
       </c>
       <c r="C12" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>624</v>
@@ -13326,103 +14680,103 @@
         <v>624</v>
       </c>
       <c r="G12" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B13" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C13" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>624</v>
-      </c>
-      <c r="F13" t="s">
-        <v>624</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>685</v>
+        <v>629</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B14" t="s">
-        <v>666</v>
+        <v>604</v>
       </c>
       <c r="C14" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>629</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F14" t="s">
+        <v>624</v>
+      </c>
       <c r="G14" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B15" t="s">
-        <v>667</v>
+        <v>604</v>
       </c>
       <c r="C15" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>624</v>
-      </c>
-      <c r="F15" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F15" s="7"/>
       <c r="G15" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B16" t="s">
-        <v>667</v>
+        <v>604</v>
       </c>
       <c r="C16" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>629</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="G16" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="B17" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C17" t="s">
         <v>599</v>
@@ -13437,62 +14791,62 @@
         <v>624</v>
       </c>
       <c r="G17" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="B18" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C18" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>629</v>
-      </c>
-      <c r="F18" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F18" t="s">
+        <v>624</v>
+      </c>
       <c r="G18" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="B19" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C19" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>624</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F19" s="7"/>
       <c r="G19" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B20" t="s">
-        <v>607</v>
+        <v>654</v>
       </c>
       <c r="C20" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -13504,18 +14858,18 @@
         <v>624</v>
       </c>
       <c r="G20" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B21" t="s">
-        <v>607</v>
+        <v>668</v>
       </c>
       <c r="C21" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -13527,42 +14881,41 @@
         <v>624</v>
       </c>
       <c r="G21" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B22" t="s">
-        <v>607</v>
+        <v>668</v>
       </c>
       <c r="C22" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>629</v>
-      </c>
-      <c r="F22" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F22" t="s">
+        <v>624</v>
+      </c>
       <c r="G22" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>609</v>
-      </c>
-      <c r="B23" t="s">
-        <v>654</v>
+        <v>611</v>
       </c>
       <c r="C23" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>624</v>
@@ -13570,22 +14923,22 @@
       <c r="F23" t="s">
         <v>624</v>
       </c>
-      <c r="G23" t="s">
-        <v>638</v>
+      <c r="G23" s="12" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>610</v>
+        <v>681</v>
       </c>
       <c r="B24" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
       <c r="C24" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>624</v>
@@ -13593,16 +14946,16 @@
       <c r="F24" t="s">
         <v>624</v>
       </c>
-      <c r="G24" t="s">
-        <v>639</v>
+      <c r="G24" s="12" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B25" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="C25" t="s">
         <v>597</v>
@@ -13617,18 +14970,21 @@
         <v>624</v>
       </c>
       <c r="G25" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>611</v>
+        <v>613</v>
+      </c>
+      <c r="B26" t="s">
+        <v>613</v>
       </c>
       <c r="C26" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D26">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
         <v>624</v>
@@ -13636,19 +14992,19 @@
       <c r="F26" t="s">
         <v>624</v>
       </c>
-      <c r="G26" s="12" t="s">
-        <v>684</v>
+      <c r="G26" s="13" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>681</v>
+        <v>614</v>
       </c>
       <c r="B27" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
       <c r="C27" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -13659,22 +15015,22 @@
       <c r="F27" t="s">
         <v>624</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>683</v>
+      <c r="G27" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B28" t="s">
-        <v>656</v>
+        <v>669</v>
       </c>
       <c r="C28" t="s">
         <v>597</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
         <v>624</v>
@@ -13683,41 +15039,39 @@
         <v>624</v>
       </c>
       <c r="G28" t="s">
-        <v>641</v>
+        <v>753</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>613</v>
+        <v>673</v>
       </c>
       <c r="B29" t="s">
-        <v>613</v>
+        <v>674</v>
       </c>
       <c r="C29" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>624</v>
-      </c>
-      <c r="F29" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F29" s="7"/>
       <c r="G29" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>614</v>
+        <v>673</v>
       </c>
       <c r="B30" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="C30" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -13729,21 +15083,21 @@
         <v>624</v>
       </c>
       <c r="G30" t="s">
-        <v>642</v>
+        <v>675</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B31" t="s">
-        <v>669</v>
+        <v>615</v>
       </c>
       <c r="C31" t="s">
         <v>597</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>624</v>
@@ -13752,150 +15106,150 @@
         <v>624</v>
       </c>
       <c r="G31" t="s">
-        <v>672</v>
+        <v>643</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>673</v>
+        <v>616</v>
       </c>
       <c r="B32" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
       <c r="C32" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>629</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>624</v>
+      </c>
+      <c r="F32" t="s">
+        <v>624</v>
+      </c>
       <c r="G32" t="s">
-        <v>675</v>
+        <v>644</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>673</v>
+        <v>616</v>
       </c>
       <c r="B33" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
       <c r="C33" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>624</v>
-      </c>
-      <c r="F33" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F33" s="7"/>
       <c r="G33" t="s">
-        <v>675</v>
+        <v>644</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B34" t="s">
-        <v>615</v>
+        <v>651</v>
       </c>
       <c r="C34" t="s">
         <v>597</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>624</v>
-      </c>
-      <c r="F34" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F34" s="7"/>
       <c r="G34" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B35" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C35" t="s">
         <v>599</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
         <v>624</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="7" t="s">
         <v>624</v>
       </c>
       <c r="G35" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B36" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C36" t="s">
         <v>596</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>629</v>
       </c>
       <c r="F36" s="7"/>
-      <c r="G36" t="s">
-        <v>644</v>
+      <c r="G36" s="10" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B37" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C37" t="s">
         <v>597</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>629</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" t="s">
-        <v>644</v>
+        <v>624</v>
+      </c>
+      <c r="F37" t="s">
+        <v>624</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B38" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C38" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -13903,150 +15257,83 @@
       <c r="E38" t="s">
         <v>624</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" t="s">
         <v>624</v>
       </c>
       <c r="G38" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B39" t="s">
-        <v>655</v>
+        <v>670</v>
       </c>
       <c r="C39" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>629</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="10" t="s">
-        <v>645</v>
+        <v>624</v>
+      </c>
+      <c r="F39" t="s">
+        <v>624</v>
+      </c>
+      <c r="G39" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B40" t="s">
-        <v>655</v>
+        <v>670</v>
       </c>
       <c r="C40" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>624</v>
-      </c>
-      <c r="F40" t="s">
-        <v>624</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>645</v>
+        <v>629</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B41" t="s">
-        <v>657</v>
+        <v>670</v>
       </c>
       <c r="C41" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>624</v>
-      </c>
-      <c r="F41" t="s">
-        <v>624</v>
-      </c>
+        <v>629</v>
+      </c>
+      <c r="F41" s="7"/>
       <c r="G41" t="s">
-        <v>646</v>
+        <v>676</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>619</v>
-      </c>
-      <c r="B42" t="s">
-        <v>670</v>
-      </c>
-      <c r="C42" t="s">
-        <v>599</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>624</v>
-      </c>
-      <c r="F42" t="s">
-        <v>624</v>
-      </c>
-      <c r="G42" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>619</v>
-      </c>
-      <c r="B43" t="s">
-        <v>670</v>
-      </c>
-      <c r="C43" t="s">
-        <v>596</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>629</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>619</v>
-      </c>
-      <c r="B44" t="s">
-        <v>670</v>
-      </c>
-      <c r="C44" t="s">
-        <v>597</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s">
-        <v>629</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="F45" s="8"/>
+      <c r="F42" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F26:F27 E1:E2 E34:E37 E39:E1048576 E4 G27 E6:E30">
+  <conditionalFormatting sqref="E1 E31:E34 E36:E1048576 E3 G24 E5:F27">
     <cfRule type="cellIs" dxfId="51" priority="23" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14054,7 +15341,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2 F34:F37 F39:F44 F4 G27 F6:F30">
+  <conditionalFormatting sqref="F31:F34 F36:F41 F3 G24">
     <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14062,7 +15349,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31 E33">
+  <conditionalFormatting sqref="E28 E30">
     <cfRule type="cellIs" dxfId="47" priority="19" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14070,7 +15357,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F31 F33:G33">
+  <conditionalFormatting sqref="F28 F30:G30">
     <cfRule type="cellIs" dxfId="45" priority="17" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14078,7 +15365,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E29">
     <cfRule type="cellIs" dxfId="43" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14086,7 +15373,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
+  <conditionalFormatting sqref="F29">
     <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14094,7 +15381,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
+  <conditionalFormatting sqref="E35">
     <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14102,7 +15389,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
+  <conditionalFormatting sqref="F35">
     <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14110,7 +15397,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E2">
     <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14118,7 +15405,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
+  <conditionalFormatting sqref="F2">
     <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14126,7 +15413,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
+  <conditionalFormatting sqref="E4">
     <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14134,7 +15421,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -14146,12 +15433,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D7293A-2FDE-C04B-953B-A96561E14327}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>